<commit_message>
updated the Excel table that summarizes results, to take into account that now FGMRES is used rather than GCR. Convergence is generally faster than previous.
Yet, there are some interested cases for which convergence rather suddenly seems to stall. 

git-svn-id: svn+ssh://gaia.geo.uni-mainz.de/local/home/lkausb/svn/LaMEM/trunk@5693 26174531-3d5a-4d31-aba0-7a6658d032cb
</commit_message>
<xml_diff>
--- a/input_models/FB_tests_canonical/FB_vs_MultipleSpheres.xlsx
+++ b/input_models/FB_tests_canonical/FB_vs_MultipleSpheres.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Testing the effect of VC and geometry setup for simulations in which we use either a single falling block or 8 multiple spheres</t>
   </si>
@@ -39,15 +39,9 @@
     <t>Total solve [s]</t>
   </si>
   <si>
-    <t>Coupled MG, with GMRES/BJACOBI at coarse level solved to 1e-5 precision and GMRES/Jacobi(20,20) smoothers and GCR outer iteration and 64^3 resolution, using 4 CPUs; 5 GMG levels</t>
-  </si>
-  <si>
     <t>&gt;1000</t>
   </si>
   <si>
-    <t>Setup:</t>
-  </si>
-  <si>
     <t>Setup:FallingBlock_canonical_BlockMG_accurateCoarse.dat and MultipleSpheres_canonical_BlockMG_accurateCoarse.dat</t>
   </si>
   <si>
@@ -63,28 +57,28 @@
     <t>We reproduce the setup described in the pTatin SC paper of May et al. (2014) with  the same parameters, running the sim for 1 timesteps</t>
   </si>
   <si>
-    <t>Blocked matrix and MG, with GMRES/BJACOBI at coarse level solved to 1e-5 precision and GMRES/Jacobi(20,20) smoothers and GCR outer iteration(rtol 1e-5) and 32^3 resolution, using 4 CPUs; 5 GMG levels</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>&gt;3000</t>
-  </si>
-  <si>
     <t>COUPLED MG with -pcmat_no_dev_proj option</t>
   </si>
   <si>
     <t>COUPLED MG without -pcmat_no_dev_proj option</t>
   </si>
   <si>
-    <t>STALLS</t>
-  </si>
-  <si>
     <t>COUPLED MG with -pcmat_no_dev_proj option but computing viscosity contrast by having a matrix viscosity 1 and block viscosity as indicated</t>
   </si>
   <si>
-    <t xml:space="preserve">STALLS </t>
+    <t>Coupled MG, with GMRES/BJACOBI at coarse level solved to 1e-5 precision and GMRES/Jacobi(20,20) smoothers and FGMRES outer iteration and 32^3 resolution, using 4 CPUs; 5 GMG levels</t>
+  </si>
+  <si>
+    <t>Setup: FallingBlock_canonical_BlockMG_accurateCoarse.dat and MultipleSpheres_canonical_BlockMG_accurateCoarse.dat</t>
+  </si>
+  <si>
+    <t>Blocked matrix and MG, with GMRES/BJACOBI at coarse level solved to 1e-5 precision and GMRES/Jacobi(20,20) smoothers and FGMRES outer iteration(rtol 1e-5) and 32^3 resolution, using 4 CPUs; 5 GMG levels</t>
+  </si>
+  <si>
+    <t>&gt;5000</t>
   </si>
 </sst>
 </file>
@@ -191,7 +185,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -215,8 +209,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -231,8 +237,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -244,6 +253,12 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -255,6 +270,12 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -584,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M30"/>
+  <dimension ref="A2:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -599,6 +620,7 @@
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13">
@@ -608,33 +630,33 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="C10" s="9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -646,14 +668,14 @@
         <v>3</v>
       </c>
       <c r="E11" s="6"/>
-      <c r="H11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" s="4"/>
-      <c r="L11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M11" s="4"/>
+      <c r="H11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="L11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="7" t="s">
@@ -674,37 +696,30 @@
       <c r="H12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="I12" s="2"/>
       <c r="L12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="M12" s="2"/>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="8">
         <v>1</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C13">
-        <v>0.81</v>
+        <v>0.96</v>
       </c>
       <c r="D13">
         <v>6</v>
       </c>
       <c r="E13">
-        <v>0.82</v>
+        <v>0.84</v>
       </c>
       <c r="H13">
         <v>6</v>
-      </c>
-      <c r="I13">
-        <v>0.79</v>
       </c>
       <c r="L13">
         <v>6</v>
@@ -715,22 +730,19 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>1.24</v>
+        <v>1.78</v>
       </c>
       <c r="D14">
         <v>11</v>
       </c>
       <c r="E14">
-        <v>1.32</v>
+        <v>1.27</v>
       </c>
       <c r="H14">
-        <v>10</v>
-      </c>
-      <c r="I14">
-        <v>1.2549999999999999</v>
+        <v>11</v>
       </c>
       <c r="L14">
         <v>9</v>
@@ -741,10 +753,10 @@
         <v>100</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C15">
-        <v>1.65</v>
+        <v>2.2959999999999998</v>
       </c>
       <c r="D15">
         <v>20</v>
@@ -753,13 +765,10 @@
         <v>2.21</v>
       </c>
       <c r="H15">
-        <v>15</v>
-      </c>
-      <c r="I15">
-        <v>1.73</v>
+        <v>20</v>
       </c>
       <c r="L15">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -767,69 +776,83 @@
         <v>1000</v>
       </c>
       <c r="B16">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C16">
-        <v>3.21</v>
+        <v>3.3279999999999998</v>
       </c>
       <c r="D16">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E16">
-        <v>5.16</v>
+        <v>4.41</v>
       </c>
       <c r="H16">
-        <v>109</v>
-      </c>
-      <c r="I16">
-        <v>11.5</v>
+        <v>43</v>
       </c>
       <c r="L16">
-        <v>19</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="8">
         <v>10000</v>
       </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B17">
+        <v>47</v>
+      </c>
+      <c r="C17">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D17">
+        <v>168</v>
+      </c>
+      <c r="E17">
+        <v>17.920000000000002</v>
+      </c>
+      <c r="H17">
+        <v>168</v>
+      </c>
+      <c r="L17">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="12">
+        <v>100000</v>
+      </c>
+      <c r="B18">
+        <v>136</v>
+      </c>
+      <c r="C18">
+        <v>13.69</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="H17" t="s">
-        <v>7</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="H18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="L17">
-        <v>144</v>
+      <c r="L18">
+        <v>1258</v>
       </c>
     </row>
     <row r="21" spans="1:12">
       <c r="A21" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:12">
       <c r="A22" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:12">
       <c r="C23" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:12">
@@ -879,6 +902,12 @@
       <c r="C26">
         <v>0.86499999999999999</v>
       </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>0.85</v>
+      </c>
       <c r="H26">
         <v>3</v>
       </c>
@@ -896,11 +925,17 @@
       <c r="C27">
         <v>2.3959999999999999</v>
       </c>
+      <c r="D27">
+        <v>11</v>
+      </c>
+      <c r="E27">
+        <v>2.54</v>
+      </c>
       <c r="H27">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I27">
-        <v>3.6880000000000002</v>
+        <v>3.35</v>
       </c>
     </row>
     <row r="28" spans="1:12">
@@ -908,16 +943,22 @@
         <v>100</v>
       </c>
       <c r="B28" s="11">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C28">
-        <v>5.66</v>
+        <v>3.63</v>
+      </c>
+      <c r="D28">
+        <v>19</v>
+      </c>
+      <c r="E28">
+        <v>7.59</v>
       </c>
       <c r="H28" s="11">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="I28" s="11">
-        <v>24.4</v>
+        <v>15.9</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -925,27 +966,53 @@
         <v>1000</v>
       </c>
       <c r="B29" s="11">
-        <v>395</v>
+        <v>21</v>
       </c>
       <c r="C29">
-        <v>102</v>
+        <v>6.08</v>
+      </c>
+      <c r="D29">
+        <v>29</v>
+      </c>
+      <c r="E29">
+        <v>22.9</v>
       </c>
       <c r="H29" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I29" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="8">
         <v>10000</v>
       </c>
-      <c r="B30" t="s">
-        <v>7</v>
+      <c r="B30">
+        <v>27</v>
+      </c>
+      <c r="C30">
+        <v>10.93</v>
+      </c>
+      <c r="D30">
+        <v>54</v>
+      </c>
+      <c r="E30">
+        <v>70.3</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="12">
+        <v>100000</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1) Updated the coupled MG tests as something must have been wrong before (I could not reproduce the numbers in the table).
2) Added Anton’s favorite CoupledMG options for the Falling Block and 8-Spheres setup (with a direct coarse grid solver). 
The results also confirm the importance of using the -pcmat_no_dev_proj option at all times, and show how the spheres setup is more tricky to solve than the FB setup.

git-svn-id: svn+ssh://gaia.geo.uni-mainz.de/local/home/lkausb/svn/LaMEM/trunk@5705 26174531-3d5a-4d31-aba0-7a6658d032cb
</commit_message>
<xml_diff>
--- a/input_models/FB_tests_canonical/FB_vs_MultipleSpheres.xlsx
+++ b/input_models/FB_tests_canonical/FB_vs_MultipleSpheres.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
   <si>
     <t>Testing the effect of VC and geometry setup for simulations in which we use either a single falling block or 8 multiple spheres</t>
   </si>
@@ -78,7 +78,13 @@
     <t>Blocked matrix and MG, with GMRES/BJACOBI at coarse level solved to 1e-5 precision and GMRES/Jacobi(20,20) smoothers and FGMRES outer iteration(rtol 1e-5) and 32^3 resolution, using 4 CPUs; 5 GMG levels</t>
   </si>
   <si>
-    <t>&gt;5000</t>
+    <t>Coupled MG with Anton's favorite solver options</t>
+  </si>
+  <si>
+    <t>Setup: FallingBlock_canonical_coupledMG_directCoarse.dat and MultipleSpheres_canonical_coupledMG_directCoarse.dat</t>
+  </si>
+  <si>
+    <t>25?</t>
   </si>
 </sst>
 </file>
@@ -185,8 +191,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -241,7 +265,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -259,6 +283,15 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -276,6 +309,15 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -605,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M31"/>
+  <dimension ref="A2:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -713,16 +755,16 @@
         <v>0.96</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E13">
-        <v>0.84</v>
+        <v>1.07</v>
       </c>
       <c r="H13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L13">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -736,16 +778,16 @@
         <v>1.78</v>
       </c>
       <c r="D14">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E14">
-        <v>1.27</v>
+        <v>2.12</v>
       </c>
       <c r="H14">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="L14">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -759,16 +801,16 @@
         <v>2.2959999999999998</v>
       </c>
       <c r="D15">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="E15">
-        <v>2.21</v>
+        <v>3.58</v>
       </c>
       <c r="H15">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="L15">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -782,16 +824,16 @@
         <v>3.3279999999999998</v>
       </c>
       <c r="D16">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="E16">
-        <v>4.41</v>
+        <v>7.82</v>
       </c>
       <c r="H16">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="L16">
-        <v>48</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:12">
@@ -805,16 +847,16 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D17">
-        <v>168</v>
+        <v>270</v>
       </c>
       <c r="E17">
-        <v>17.920000000000002</v>
+        <v>31.2</v>
       </c>
       <c r="H17">
-        <v>168</v>
+        <v>339</v>
       </c>
       <c r="L17">
-        <v>175</v>
+        <v>341</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -828,13 +870,13 @@
         <v>13.69</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="L18">
-        <v>1258</v>
+        <v>1517</v>
       </c>
     </row>
     <row r="21" spans="1:12">
@@ -1013,6 +1055,171 @@
       </c>
       <c r="H31" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="C38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L38" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="B39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="4"/>
+      <c r="D39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" s="6"/>
+      <c r="H39" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L39" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="8">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="H41">
+        <v>7</v>
+      </c>
+      <c r="L41">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="8">
+        <v>10</v>
+      </c>
+      <c r="B42">
+        <v>11</v>
+      </c>
+      <c r="D42">
+        <v>12</v>
+      </c>
+      <c r="H42">
+        <v>12</v>
+      </c>
+      <c r="L42">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="8">
+        <v>100</v>
+      </c>
+      <c r="B43">
+        <v>12</v>
+      </c>
+      <c r="D43">
+        <v>19</v>
+      </c>
+      <c r="H43">
+        <v>19</v>
+      </c>
+      <c r="L43">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="8">
+        <v>1000</v>
+      </c>
+      <c r="B44">
+        <v>13</v>
+      </c>
+      <c r="D44">
+        <v>39</v>
+      </c>
+      <c r="H44">
+        <v>41</v>
+      </c>
+      <c r="L44">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="8">
+        <v>10000</v>
+      </c>
+      <c r="B45">
+        <v>17</v>
+      </c>
+      <c r="D45">
+        <v>80</v>
+      </c>
+      <c r="H45">
+        <v>141</v>
+      </c>
+      <c r="L45">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="12">
+        <v>100000</v>
+      </c>
+      <c r="B46">
+        <v>26</v>
+      </c>
+      <c r="D46" s="11">
+        <v>88</v>
+      </c>
+      <c r="E46">
+        <v>5.51</v>
+      </c>
+      <c r="H46">
+        <v>585</v>
+      </c>
+      <c r="L46" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added test results for cases with and w/out null space attached at the coarse level solver (using GAMG as a solver). Attaching the nullspace is generally faster, and is particularly important for the CoupledMG solver
git-svn-id: svn+ssh://gaia.geo.uni-mainz.de/local/home/lkausb/svn/LaMEM/trunk@5708 26174531-3d5a-4d31-aba0-7a6658d032cb
</commit_message>
<xml_diff>
--- a/input_models/FB_tests_canonical/FB_vs_MultipleSpheres.xlsx
+++ b/input_models/FB_tests_canonical/FB_vs_MultipleSpheres.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Testing the effect of VC and geometry setup for simulations in which we use either a single falling block or 8 multiple spheres</t>
   </si>
@@ -85,6 +85,48 @@
   </si>
   <si>
     <t>25?</t>
+  </si>
+  <si>
+    <t>Not attached</t>
+  </si>
+  <si>
+    <t>VC 1e4; 32^3</t>
+  </si>
+  <si>
+    <t>VC 1e4; 64^3</t>
+  </si>
+  <si>
+    <t>Attached</t>
+  </si>
+  <si>
+    <t>Effect of attaching or not attaching the nullspace to the convergence rate. Numbers refer to the release of LaMEM. r5698 - not attached; r.5707 - attached; We do a 8-sphere setup with VC 1e4 and report # of iterations</t>
+  </si>
+  <si>
+    <t>&gt;500</t>
+  </si>
+  <si>
+    <t>COUPLED MG; GMRES/GAMG coarse grid solver</t>
+  </si>
+  <si>
+    <t>VC 1e4; 128*64*64</t>
+  </si>
+  <si>
+    <t>&gt;100</t>
+  </si>
+  <si>
+    <t>VC 1e5; 32^3</t>
+  </si>
+  <si>
+    <t>VC 1e5; 64^3</t>
+  </si>
+  <si>
+    <t>BLOCKED MG; GMRES/GAMG coarse grid solver</t>
+  </si>
+  <si>
+    <t>Tests are done with the file MultipleSpheres_canonical_coupledMG_accurateCoarse.dat  and MultipleSpheres_canonical_coupledMG_directCoarse.dat with GAMG solver switched on</t>
+  </si>
+  <si>
+    <t>&gt;200</t>
   </si>
 </sst>
 </file>
@@ -156,7 +198,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +223,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -191,7 +239,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -245,8 +293,32 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -264,8 +336,9 @@
     <xf numFmtId="11" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="77">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -292,6 +365,18 @@
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -318,6 +403,18 @@
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -647,17 +744,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M46"/>
+  <dimension ref="A2:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
     <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
     <col min="8" max="8" width="13.5" customWidth="1"/>
@@ -1220,6 +1317,123 @@
       </c>
       <c r="L46" s="10" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="B55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="B56" t="s">
+        <v>22</v>
+      </c>
+      <c r="C56" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" t="s">
+        <v>22</v>
+      </c>
+      <c r="F56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B57">
+        <v>80</v>
+      </c>
+      <c r="C57">
+        <v>80</v>
+      </c>
+      <c r="E57">
+        <v>70</v>
+      </c>
+      <c r="F57">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58">
+        <v>55</v>
+      </c>
+      <c r="E58">
+        <v>44</v>
+      </c>
+      <c r="F58">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" t="s">
+        <v>30</v>
+      </c>
+      <c r="C59">
+        <v>55</v>
+      </c>
+      <c r="E59">
+        <v>53</v>
+      </c>
+      <c r="F59">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61">
+        <v>88</v>
+      </c>
+      <c r="C61">
+        <v>88</v>
+      </c>
+      <c r="E61" t="s">
+        <v>35</v>
+      </c>
+      <c r="F61" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62">
+        <v>316</v>
+      </c>
+      <c r="C62">
+        <v>230</v>
+      </c>
+      <c r="E62" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>